<commit_message>
Mon Dec  9 05:10:52 PM EST 2024
</commit_message>
<xml_diff>
--- a/ozone/ozone_MB_params.xlsx
+++ b/ozone/ozone_MB_params.xlsx
@@ -487,7 +487,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.001</v>
+        <v>1e-06</v>
       </c>
     </row>
     <row r="7">
@@ -497,7 +497,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.001</v>
+        <v>1e-06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>